<commit_message>
OCHRE to REopt posts
</commit_message>
<xml_diff>
--- a/nova_metrics/tests/test OCHRE/Inputs.xlsx
+++ b/nova_metrics/tests/test OCHRE/Inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean\Dropbox\NREL Work\Year 2020\NOVA\test OCHRE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean\Dropbox\NREL Work\Year 2020\NOVA\Metrics at Scale\nova_metrics\tests\test OCHRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F4EDCB8-DAB4-4D17-9F87-691F3C254C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA33D06B-E366-41DF-B799-555F1E8175A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{781F73DF-6059-4588-90B8-13D682197959}"/>
+    <workbookView xWindow="-28920" yWindow="-150" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{781F73DF-6059-4588-90B8-13D682197959}"/>
   </bookViews>
   <sheets>
     <sheet name="File Paths" sheetId="2" r:id="rId1"/>
@@ -38,14 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>post_name</t>
   </si>
   <si>
-    <t>output_subfolder</t>
-  </si>
-  <si>
     <t>PV|max_kw</t>
   </si>
   <si>
@@ -190,37 +187,37 @@
     <t>ochre_value</t>
   </si>
   <si>
-    <t>ochre_main_folder</t>
-  </si>
-  <si>
     <t>OCHRE Outputs</t>
   </si>
   <si>
     <t>properties_file</t>
   </si>
   <si>
-    <t>_rc_model.properties</t>
-  </si>
-  <si>
     <t>hourly_inputs</t>
   </si>
   <si>
-    <t>lunit_dispatchableloads_fixedtech</t>
-  </si>
-  <si>
-    <t>lunit_dispatchableloads</t>
-  </si>
-  <si>
-    <t>lunit_hvac_only</t>
-  </si>
-  <si>
-    <t>McKnight_Lane_LUnit_2019</t>
-  </si>
-  <si>
     <t xml:space="preserve"> reopt_root_url</t>
   </si>
   <si>
-    <t>Unit_2019_subset.csv</t>
+    <t>ochre_outputs_main_folder</t>
+  </si>
+  <si>
+    <t>ochre_inputs_main_folder</t>
+  </si>
+  <si>
+    <t>OCHRE Inputs</t>
+  </si>
+  <si>
+    <t>OCHRE_Run.csv</t>
+  </si>
+  <si>
+    <t>_house.yaml</t>
+  </si>
+  <si>
+    <t>dispatchable_loads</t>
+  </si>
+  <si>
+    <t>Building 1</t>
   </si>
 </sst>
 </file>
@@ -265,10 +262,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
@@ -596,74 +592,74 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
         <v>43</v>
-      </c>
-      <c r="B8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -676,44 +672,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3909B4FE-AA3A-42BB-BD56-AAFC263B8137}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -723,296 +730,162 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C68F83-40BB-4EE0-A7A7-91AB6EDE70E1}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="4"/>
+    <col min="1" max="1" width="24" style="2" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="3">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3">
-        <v>5</v>
-      </c>
-      <c r="I3" s="3">
-        <v>5</v>
-      </c>
-      <c r="J3" s="3">
-        <v>5</v>
-      </c>
-      <c r="K3" s="3">
-        <v>10</v>
-      </c>
-      <c r="L3" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <v>1000</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1000</v>
-      </c>
-      <c r="K4" s="3">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3">
-        <v>1000</v>
-      </c>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="4">
-        <v>5</v>
-      </c>
-      <c r="H6" s="4">
-        <v>5</v>
-      </c>
-      <c r="I6" s="4">
-        <v>5</v>
-      </c>
-      <c r="J6" s="4">
-        <v>5</v>
-      </c>
-      <c r="K6" s="4">
-        <v>10</v>
-      </c>
-      <c r="L6" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="F7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="E14"/>
-      <c r="F14"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11"/>
+      <c r="D11"/>
+      <c r="E11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1035,70 +908,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1118,34 +991,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>